<commit_message>
Update several sections in the CW3M Digital Handbook.
</commit_message>
<xml_diff>
--- a/DataCW3M/SkillAssessment/StatisticsCalculator108months.xlsx
+++ b/DataCW3M/SkillAssessment/StatisticsCalculator108months.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\SkillAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39AF5E3-ABB4-4D51-9B8C-2EB3A1CDCAE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E3A86A-DCBD-4AA3-8F5A-8240B4A1A962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics calculator" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Month index</t>
   </si>
@@ -55,18 +55,6 @@
   </si>
   <si>
     <t>R2</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>std dev</t>
-  </si>
-  <si>
-    <t>gage</t>
-  </si>
-  <si>
-    <t>gage SD</t>
   </si>
   <si>
     <t>O-P</t>
@@ -144,9 +132,6 @@
     <t>obs</t>
   </si>
   <si>
-    <t>sim minus obs</t>
-  </si>
-  <si>
     <t>C139</t>
   </si>
   <si>
@@ -154,6 +139,30 @@
   </si>
   <si>
     <t>C141+ minus C139</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>std dev P</t>
+  </si>
+  <si>
+    <t>std dev O</t>
+  </si>
+  <si>
+    <t>Obar</t>
+  </si>
+  <si>
+    <t>Pbar</t>
+  </si>
+  <si>
+    <t>Pbar - Obar</t>
+  </si>
+  <si>
+    <t>abs(P-O)</t>
+  </si>
+  <si>
+    <t>MAE</t>
   </si>
 </sst>
 </file>
@@ -643,7 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -658,7 +667,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3340,16 +3348,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>430530</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2713671</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>453390</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>77151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>60959</xdr:rowOff>
+      <xdr:colOff>674370</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>167639</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3717,8 +3725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD3290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I111"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3738,26 +3746,26 @@
       <c r="H1"/>
       <c r="I1"/>
       <c r="S1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="T1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="U1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:30" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="9">
+        <v>41</v>
+      </c>
+      <c r="B2" s="8">
         <f>H2-I2</f>
         <v>0.82378943518518799</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -3776,9 +3784,15 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="P2" s="4">
+        <f>AVERAGE(P4:P111)</f>
+        <v>2.1646616809840462</v>
+      </c>
       <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="R2" s="4">
+        <f>AVERAGE(R4:R111)</f>
+        <v>1.1491599166666662</v>
+      </c>
       <c r="S2">
         <f>AVERAGE(S4:S111)</f>
         <v>8.4489025648148157</v>
@@ -3812,72 +3826,74 @@
         <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="4"/>
+      <c r="R3" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="S3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="Z3" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="1">
         <f>1-SUM(P4:P111)/SUM(M4:M111)</f>
         <v>0.63532077747348414</v>
       </c>
@@ -3932,6 +3948,10 @@
         <f>(I4-H$2)*(I4-H$2)</f>
         <v>6.2447526296362144</v>
       </c>
+      <c r="R4" s="2">
+        <f>ABS(J4)</f>
+        <v>0.52779000000000043</v>
+      </c>
       <c r="S4">
         <v>5.1376660000000003</v>
       </c>
@@ -3969,7 +3989,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="1">
         <f>SQRT(SUM(P4:P111))/SQRT(SUM(Q4:Q111))</f>
         <v>0.57206970086927267</v>
       </c>
@@ -4024,6 +4044,10 @@
         <f t="shared" ref="Q5:Q68" si="7">(I5-H$2)*(I5-H$2)</f>
         <v>8.1564235883248291</v>
       </c>
+      <c r="R5" s="2">
+        <f t="shared" ref="R5:R68" si="8">ABS(J5)</f>
+        <v>8.3349999999997593E-3</v>
+      </c>
       <c r="S5">
         <v>5.2818040000000002</v>
       </c>
@@ -4031,7 +4055,7 @@
         <v>5.7384250000000003</v>
       </c>
       <c r="U5">
-        <f t="shared" ref="U5:U68" si="8">T5-S5</f>
+        <f t="shared" ref="U5:U68" si="9">T5-S5</f>
         <v>0.45662100000000017</v>
       </c>
       <c r="V5"/>
@@ -4061,7 +4085,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="1">
         <f>B12*B12</f>
         <v>0.91363722685536253</v>
       </c>
@@ -4116,6 +4140,10 @@
         <f t="shared" si="7"/>
         <v>8.8216205697150496</v>
       </c>
+      <c r="R6" s="2">
+        <f t="shared" si="8"/>
+        <v>0.50546399999999991</v>
+      </c>
       <c r="S6">
         <v>5.855613</v>
       </c>
@@ -4123,7 +4151,7 @@
         <v>6.4123729999999997</v>
       </c>
       <c r="U6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.5567599999999997</v>
       </c>
       <c r="V6"/>
@@ -4151,9 +4179,9 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="8">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1">
         <f>H2</f>
         <v>8.0600743055555579</v>
       </c>
@@ -4208,6 +4236,10 @@
         <f t="shared" si="7"/>
         <v>7.1660575845143857</v>
       </c>
+      <c r="R7" s="2">
+        <f t="shared" si="8"/>
+        <v>0.59845799999999993</v>
+      </c>
       <c r="S7">
         <v>6.2127059999999998</v>
       </c>
@@ -4215,7 +4247,7 @@
         <v>6.5012179999999997</v>
       </c>
       <c r="U7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.28851199999999988</v>
       </c>
       <c r="V7"/>
@@ -4243,9 +4275,9 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="8">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1">
         <f>_xlfn.STDEV.P(H4:H111)</f>
         <v>3.3153796901639776</v>
       </c>
@@ -4300,6 +4332,10 @@
         <f t="shared" si="7"/>
         <v>2.5812577254699334</v>
       </c>
+      <c r="R8" s="2">
+        <f t="shared" si="8"/>
+        <v>0.54995499999999975</v>
+      </c>
       <c r="S8">
         <v>6.9663380000000004</v>
       </c>
@@ -4307,7 +4343,7 @@
         <v>7.5264199999999999</v>
       </c>
       <c r="U8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.56008199999999952</v>
       </c>
       <c r="V8"/>
@@ -4335,9 +4371,9 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="8">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1">
         <f>I2</f>
         <v>7.2362848703703699</v>
       </c>
@@ -4392,6 +4428,10 @@
         <f t="shared" si="7"/>
         <v>0.55714086741614488</v>
       </c>
+      <c r="R9" s="2">
+        <f t="shared" si="8"/>
+        <v>0.35575200000000073</v>
+      </c>
       <c r="S9">
         <v>8.0567130000000002</v>
       </c>
@@ -4399,7 +4439,7 @@
         <v>9.3709589999999992</v>
       </c>
       <c r="U9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3142459999999989</v>
       </c>
       <c r="V9"/>
@@ -4427,9 +4467,9 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="8">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1">
         <f>_xlfn.STDEV.P(I4:I111)</f>
         <v>2.4363490262215648</v>
       </c>
@@ -4483,6 +4523,10 @@
         <f t="shared" si="7"/>
         <v>10.199851874122691</v>
       </c>
+      <c r="R10" s="2">
+        <f t="shared" si="8"/>
+        <v>1.5955259999999996</v>
+      </c>
       <c r="S10">
         <v>10.862743</v>
       </c>
@@ -4490,7 +4534,7 @@
         <v>12.556028</v>
       </c>
       <c r="U10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6932849999999995</v>
       </c>
       <c r="V10"/>
@@ -4517,6 +4561,13 @@
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1">
+        <f>SQRT(P$2)</f>
+        <v>1.4712789269829314</v>
+      </c>
       <c r="D11">
         <v>7</v>
       </c>
@@ -4567,6 +4618,10 @@
         <f t="shared" si="7"/>
         <v>7.0993134898386332</v>
       </c>
+      <c r="R11" s="2">
+        <f t="shared" si="8"/>
+        <v>2.0117980000000006</v>
+      </c>
       <c r="S11">
         <v>13.279059</v>
       </c>
@@ -4574,7 +4629,7 @@
         <v>15.188703</v>
       </c>
       <c r="U11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9096440000000001</v>
       </c>
       <c r="V11"/>
@@ -4602,9 +4657,9 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="7">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
         <f>SUM(O4:O111)/SQRT(SUM(M4:M111)*SUM(N4:N111))</f>
         <v>0.95584372512213656</v>
       </c>
@@ -4659,6 +4714,10 @@
         <f t="shared" si="7"/>
         <v>1.7702746741953663</v>
       </c>
+      <c r="R12" s="2">
+        <f t="shared" si="8"/>
+        <v>0.87713899999999967</v>
+      </c>
       <c r="S12">
         <v>13.139711999999999</v>
       </c>
@@ -4666,7 +4725,7 @@
         <v>15.156300999999999</v>
       </c>
       <c r="U12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0165889999999997</v>
       </c>
       <c r="V12"/>
@@ -4693,6 +4752,13 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2">
+        <f>P2</f>
+        <v>2.1646616809840462</v>
+      </c>
       <c r="D13">
         <v>9</v>
       </c>
@@ -4743,6 +4809,10 @@
         <f t="shared" si="7"/>
         <v>8.9521421246150257E-2</v>
       </c>
+      <c r="R13" s="2">
+        <f t="shared" si="8"/>
+        <v>0.13175999999999988</v>
+      </c>
       <c r="S13">
         <v>12.061854</v>
       </c>
@@ -4750,7 +4820,7 @@
         <v>14.002096</v>
       </c>
       <c r="U13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9402419999999996</v>
       </c>
       <c r="V13"/>
@@ -4827,6 +4897,10 @@
         <f t="shared" si="7"/>
         <v>5.2636991776820468</v>
       </c>
+      <c r="R14" s="2">
+        <f t="shared" si="8"/>
+        <v>0.87618600000000058</v>
+      </c>
       <c r="S14">
         <v>5.7312029999999998</v>
       </c>
@@ -4834,7 +4908,7 @@
         <v>6.2288560000000004</v>
       </c>
       <c r="U14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.49765300000000057</v>
       </c>
       <c r="V14"/>
@@ -4911,6 +4985,10 @@
         <f t="shared" si="7"/>
         <v>10.615602060378274</v>
       </c>
+      <c r="R15" s="2">
+        <f t="shared" si="8"/>
+        <v>0.63796500000000034</v>
+      </c>
       <c r="S15">
         <v>4.0966670000000001</v>
       </c>
@@ -4918,7 +4996,7 @@
         <v>3.8112159999999999</v>
       </c>
       <c r="U15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.28545100000000012</v>
       </c>
       <c r="V15"/>
@@ -4995,6 +5073,10 @@
         <f t="shared" si="7"/>
         <v>14.101799710562554</v>
       </c>
+      <c r="R16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.3421479999999999</v>
+      </c>
       <c r="S16">
         <v>4.0692149999999998</v>
       </c>
@@ -5002,7 +5084,7 @@
         <v>4.1087809999999996</v>
       </c>
       <c r="U16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.9565999999999768E-2</v>
       </c>
       <c r="V16"/>
@@ -5058,6 +5140,10 @@
         <f t="shared" si="7"/>
         <v>20.043146715767286</v>
       </c>
+      <c r="R17" s="2">
+        <f t="shared" si="8"/>
+        <v>0.69598000000000004</v>
+      </c>
       <c r="S17">
         <v>4.3104899999999997</v>
       </c>
@@ -5065,7 +5151,7 @@
         <v>4.5162529999999999</v>
       </c>
       <c r="U17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20576300000000014</v>
       </c>
       <c r="V17"/>
@@ -5121,6 +5207,10 @@
         <f t="shared" si="7"/>
         <v>12.496502891822722</v>
       </c>
+      <c r="R18" s="2">
+        <f t="shared" si="8"/>
+        <v>0.28498000000000001</v>
+      </c>
       <c r="S18">
         <v>4.6696390000000001</v>
       </c>
@@ -5128,7 +5218,7 @@
         <v>4.4694390000000004</v>
       </c>
       <c r="U18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.20019999999999971</v>
       </c>
       <c r="V18"/>
@@ -5184,6 +5274,10 @@
         <f t="shared" si="7"/>
         <v>10.294551214901439</v>
       </c>
+      <c r="R19" s="2">
+        <f t="shared" si="8"/>
+        <v>0.31367399999999979</v>
+      </c>
       <c r="S19">
         <v>5.725752</v>
       </c>
@@ -5191,7 +5285,7 @@
         <v>6.1887270000000001</v>
       </c>
       <c r="U19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.46297500000000014</v>
       </c>
       <c r="V19"/>
@@ -5247,6 +5341,10 @@
         <f t="shared" si="7"/>
         <v>4.9640566578214376</v>
       </c>
+      <c r="R20" s="2">
+        <f t="shared" si="8"/>
+        <v>0.74002500000000015</v>
+      </c>
       <c r="S20">
         <v>6.651535</v>
       </c>
@@ -5254,7 +5352,7 @@
         <v>7.3997349999999997</v>
       </c>
       <c r="U20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.74819999999999975</v>
       </c>
       <c r="V20"/>
@@ -5310,6 +5408,10 @@
         <f t="shared" si="7"/>
         <v>0.11644699358648403</v>
       </c>
+      <c r="R21" s="2">
+        <f t="shared" si="8"/>
+        <v>1.2883189999999995</v>
+      </c>
       <c r="S21">
         <v>8.1925410000000003</v>
       </c>
@@ -5317,7 +5419,7 @@
         <v>9.4273530000000001</v>
       </c>
       <c r="U21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2348119999999998</v>
       </c>
       <c r="V21"/>
@@ -5373,6 +5475,10 @@
         <f t="shared" si="7"/>
         <v>5.8107980404800843</v>
       </c>
+      <c r="R22" s="2">
+        <f t="shared" si="8"/>
+        <v>1.1445179999999997</v>
+      </c>
       <c r="S22">
         <v>10.529388000000001</v>
       </c>
@@ -5380,7 +5486,7 @@
         <v>12.164102</v>
       </c>
       <c r="U22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6347139999999989</v>
       </c>
       <c r="V22"/>
@@ -5436,6 +5542,10 @@
         <f t="shared" si="7"/>
         <v>6.3177510921597522</v>
       </c>
+      <c r="R23" s="2">
+        <f t="shared" si="8"/>
+        <v>2.5068619999999999</v>
+      </c>
       <c r="S23">
         <v>12.893722</v>
       </c>
@@ -5443,7 +5553,7 @@
         <v>14.740093</v>
       </c>
       <c r="U23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.8463709999999995</v>
       </c>
       <c r="V23"/>
@@ -5499,6 +5609,10 @@
         <f t="shared" si="7"/>
         <v>1.7707803066392551</v>
       </c>
+      <c r="R24" s="2">
+        <f t="shared" si="8"/>
+        <v>2.8465779999999992</v>
+      </c>
       <c r="S24">
         <v>13.478433000000001</v>
       </c>
@@ -5506,7 +5620,7 @@
         <v>15.472922000000001</v>
       </c>
       <c r="U24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9944889999999997</v>
       </c>
       <c r="V24"/>
@@ -5562,6 +5676,10 @@
         <f t="shared" si="7"/>
         <v>0.28162689353259579</v>
       </c>
+      <c r="R25" s="2">
+        <f t="shared" si="8"/>
+        <v>0.53421799999999919</v>
+      </c>
       <c r="S25">
         <v>12.416278</v>
       </c>
@@ -5569,7 +5687,7 @@
         <v>14.415647999999999</v>
       </c>
       <c r="U25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.999369999999999</v>
       </c>
       <c r="V25"/>
@@ -5625,6 +5743,10 @@
         <f t="shared" si="7"/>
         <v>7.6134898412364969</v>
       </c>
+      <c r="R26" s="2">
+        <f t="shared" si="8"/>
+        <v>0.41707999999999945</v>
+      </c>
       <c r="S26">
         <v>7.2547030000000001</v>
       </c>
@@ -5632,7 +5754,7 @@
         <v>8.0990950000000002</v>
       </c>
       <c r="U26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.84439200000000003</v>
       </c>
       <c r="V26"/>
@@ -5688,6 +5810,10 @@
         <f t="shared" si="7"/>
         <v>20.580315894147056</v>
       </c>
+      <c r="R27" s="2">
+        <f t="shared" si="8"/>
+        <v>0.87391599999999992</v>
+      </c>
       <c r="S27">
         <v>3.306524</v>
       </c>
@@ -5695,7 +5821,7 @@
         <v>3.2822840000000002</v>
       </c>
       <c r="U27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.4239999999999817E-2</v>
       </c>
       <c r="V27"/>
@@ -5751,6 +5877,10 @@
         <f t="shared" si="7"/>
         <v>14.91418128458678</v>
       </c>
+      <c r="R28" s="2">
+        <f t="shared" si="8"/>
+        <v>0.23610700000000051</v>
+      </c>
       <c r="S28">
         <v>4.1439440000000003</v>
       </c>
@@ -5758,7 +5888,7 @@
         <v>3.927359</v>
       </c>
       <c r="U28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.21658500000000025</v>
       </c>
       <c r="V28"/>
@@ -5814,6 +5944,10 @@
         <f t="shared" si="7"/>
         <v>14.468075155342554</v>
       </c>
+      <c r="R29" s="2">
+        <f t="shared" si="8"/>
+        <v>0.21223599999999987</v>
+      </c>
       <c r="S29">
         <v>4.8668040000000001</v>
       </c>
@@ -5821,7 +5955,7 @@
         <v>5.1388389999999999</v>
       </c>
       <c r="U29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.2720349999999998</v>
       </c>
       <c r="V29"/>
@@ -5877,6 +6011,10 @@
         <f t="shared" si="7"/>
         <v>14.137715098012055</v>
       </c>
+      <c r="R30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.45946800000000021</v>
+      </c>
       <c r="S30">
         <v>4.7258519999999997</v>
       </c>
@@ -5884,7 +6022,7 @@
         <v>4.2618510000000001</v>
       </c>
       <c r="U30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.46400099999999966</v>
       </c>
       <c r="V30"/>
@@ -5940,6 +6078,10 @@
         <f t="shared" si="7"/>
         <v>7.3505311834319969</v>
       </c>
+      <c r="R31" s="2">
+        <f t="shared" si="8"/>
+        <v>1.3137410000000003</v>
+      </c>
       <c r="S31">
         <v>5.8077240000000003</v>
       </c>
@@ -5947,7 +6089,7 @@
         <v>6.2101850000000001</v>
       </c>
       <c r="U31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.40246099999999974</v>
       </c>
       <c r="V31"/>
@@ -6003,6 +6145,10 @@
         <f t="shared" si="7"/>
         <v>1.4532309866945425</v>
       </c>
+      <c r="R32" s="2">
+        <f t="shared" si="8"/>
+        <v>1.0605289999999998</v>
+      </c>
       <c r="S32">
         <v>7.3342520000000002</v>
       </c>
@@ -6010,7 +6156,7 @@
         <v>8.5556420000000006</v>
       </c>
       <c r="U32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2213900000000004</v>
       </c>
       <c r="V32"/>
@@ -6066,6 +6212,10 @@
         <f t="shared" si="7"/>
         <v>0.3534156188458687</v>
       </c>
+      <c r="R33" s="2">
+        <f t="shared" si="8"/>
+        <v>0.40677699999999994</v>
+      </c>
       <c r="S33">
         <v>8.6606909999999999</v>
       </c>
@@ -6073,7 +6223,7 @@
         <v>10.325079000000001</v>
       </c>
       <c r="U33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6643880000000006</v>
       </c>
       <c r="V33"/>
@@ -6129,6 +6279,10 @@
         <f t="shared" si="7"/>
         <v>7.6060438194490825</v>
       </c>
+      <c r="R34" s="2">
+        <f t="shared" si="8"/>
+        <v>1.834854</v>
+      </c>
       <c r="S34">
         <v>11.135647000000001</v>
       </c>
@@ -6136,7 +6290,7 @@
         <v>13.190016</v>
       </c>
       <c r="U34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0543689999999994</v>
       </c>
       <c r="V34"/>
@@ -6192,6 +6346,10 @@
         <f t="shared" si="7"/>
         <v>9.5034606213151521E-3</v>
       </c>
+      <c r="R35" s="2">
+        <f t="shared" si="8"/>
+        <v>5.4822310000000005</v>
+      </c>
       <c r="S35">
         <v>13.613049999999999</v>
       </c>
@@ -6199,7 +6357,7 @@
         <v>15.817727</v>
       </c>
       <c r="U35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.2046770000000002</v>
       </c>
       <c r="V35"/>
@@ -6255,6 +6413,10 @@
         <f t="shared" si="7"/>
         <v>1.4147691656004779</v>
       </c>
+      <c r="R36" s="2">
+        <f t="shared" si="8"/>
+        <v>2.8517510000000001</v>
+      </c>
       <c r="S36">
         <v>13.893703</v>
       </c>
@@ -6262,7 +6424,7 @@
         <v>16.177311</v>
       </c>
       <c r="U36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.2836079999999992</v>
       </c>
       <c r="V36"/>
@@ -6318,6 +6480,10 @@
         <f t="shared" si="7"/>
         <v>0.19231058301587339</v>
       </c>
+      <c r="R37" s="2">
+        <f t="shared" si="8"/>
+        <v>0.77838200000000057</v>
+      </c>
       <c r="S37">
         <v>12.509562000000001</v>
       </c>
@@ -6325,7 +6491,7 @@
         <v>14.695318</v>
       </c>
       <c r="U37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.1857559999999996</v>
       </c>
       <c r="V37"/>
@@ -6381,6 +6547,10 @@
         <f t="shared" si="7"/>
         <v>1.8228194389962109</v>
       </c>
+      <c r="R38" s="2">
+        <f t="shared" si="8"/>
+        <v>1.0471180000000002</v>
+      </c>
       <c r="S38">
         <v>6.3092430000000004</v>
       </c>
@@ -6388,7 +6558,7 @@
         <v>7.7057390000000003</v>
       </c>
       <c r="U38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.396496</v>
       </c>
       <c r="V38"/>
@@ -6444,6 +6614,10 @@
         <f t="shared" si="7"/>
         <v>9.7618022838923331</v>
       </c>
+      <c r="R39" s="2">
+        <f t="shared" si="8"/>
+        <v>1.1094349999999995</v>
+      </c>
       <c r="S39">
         <v>4.0317879999999997</v>
       </c>
@@ -6451,7 +6625,7 @@
         <v>3.4356059999999999</v>
       </c>
       <c r="U39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.59618199999999977</v>
       </c>
       <c r="V39"/>
@@ -6507,6 +6681,10 @@
         <f t="shared" si="7"/>
         <v>19.307396869557333</v>
       </c>
+      <c r="R40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.66601700000000008</v>
+      </c>
       <c r="S40">
         <v>3.631583</v>
       </c>
@@ -6514,7 +6692,7 @@
         <v>2.9708220000000001</v>
       </c>
       <c r="U40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.66076099999999993</v>
       </c>
       <c r="V40"/>
@@ -6570,6 +6748,10 @@
         <f t="shared" si="7"/>
         <v>14.071466220422055</v>
       </c>
+      <c r="R41" s="2">
+        <f t="shared" si="8"/>
+        <v>0.18199499999999968</v>
+      </c>
       <c r="S41">
         <v>4.68215</v>
       </c>
@@ -6577,7 +6759,7 @@
         <v>4.6796389999999999</v>
       </c>
       <c r="U41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.511000000000152E-3</v>
       </c>
       <c r="V41"/>
@@ -6633,6 +6815,10 @@
         <f t="shared" si="7"/>
         <v>10.178041562046332</v>
       </c>
+      <c r="R42" s="2">
+        <f t="shared" si="8"/>
+        <v>0.88638300000000037</v>
+      </c>
       <c r="S42">
         <v>5.4156449999999996</v>
       </c>
@@ -6640,7 +6826,7 @@
         <v>5.5429349999999999</v>
       </c>
       <c r="U42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.12729000000000035</v>
       </c>
       <c r="V42"/>
@@ -6696,6 +6882,10 @@
         <f t="shared" si="7"/>
         <v>5.8218514227211591</v>
       </c>
+      <c r="R43" s="2">
+        <f t="shared" si="8"/>
+        <v>0.94482899999999947</v>
+      </c>
       <c r="S43">
         <v>6.2778150000000004</v>
       </c>
@@ -6703,7 +6893,7 @@
         <v>6.8235279999999996</v>
       </c>
       <c r="U43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.54571299999999923</v>
       </c>
       <c r="V43"/>
@@ -6759,6 +6949,10 @@
         <f t="shared" si="7"/>
         <v>1.4536234035316157E-2</v>
       </c>
+      <c r="R44" s="2">
+        <f t="shared" si="8"/>
+        <v>1.0608310000000003</v>
+      </c>
       <c r="S44">
         <v>8.5226980000000001</v>
       </c>
@@ -6766,7 +6960,7 @@
         <v>9.4638559999999998</v>
       </c>
       <c r="U44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.94115799999999972</v>
       </c>
       <c r="V44"/>
@@ -6822,6 +7016,10 @@
         <f t="shared" si="7"/>
         <v>2.5148748497740878</v>
       </c>
+      <c r="R45" s="2">
+        <f t="shared" si="8"/>
+        <v>1.2528369999999995</v>
+      </c>
       <c r="S45">
         <v>9.4532790000000002</v>
       </c>
@@ -6829,7 +7027,7 @@
         <v>10.913012</v>
       </c>
       <c r="U45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.4597329999999999</v>
       </c>
       <c r="V45"/>
@@ -6885,6 +7083,10 @@
         <f t="shared" si="7"/>
         <v>10.160294552553966</v>
       </c>
+      <c r="R46" s="2">
+        <f t="shared" si="8"/>
+        <v>2.431006</v>
+      </c>
       <c r="S46">
         <v>12.156247</v>
       </c>
@@ -6892,7 +7094,7 @@
         <v>13.99469</v>
       </c>
       <c r="U46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.8384429999999998</v>
       </c>
       <c r="V46"/>
@@ -6948,6 +7150,10 @@
         <f t="shared" si="7"/>
         <v>6.0970705916542478</v>
       </c>
+      <c r="R47" s="2">
+        <f t="shared" si="8"/>
+        <v>2.7526290000000007</v>
+      </c>
       <c r="S47">
         <v>14.093671000000001</v>
       </c>
@@ -6955,7 +7161,7 @@
         <v>16.091546999999998</v>
       </c>
       <c r="U47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.997875999999998</v>
       </c>
       <c r="V47"/>
@@ -7011,6 +7217,10 @@
         <f t="shared" si="7"/>
         <v>2.3072142500556438</v>
       </c>
+      <c r="R48" s="2">
+        <f t="shared" si="8"/>
+        <v>1.0216879999999993</v>
+      </c>
       <c r="S48">
         <v>14.265325000000001</v>
       </c>
@@ -7018,7 +7228,7 @@
         <v>16.440422000000002</v>
       </c>
       <c r="U48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.1750970000000009</v>
       </c>
       <c r="V48"/>
@@ -7074,6 +7284,10 @@
         <f t="shared" si="7"/>
         <v>1.5218511325759325</v>
       </c>
+      <c r="R49" s="2">
+        <f t="shared" si="8"/>
+        <v>0.67976700000000001</v>
+      </c>
       <c r="S49">
         <v>11.068946</v>
       </c>
@@ -7081,7 +7295,7 @@
         <v>13.150365000000001</v>
       </c>
       <c r="U49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0814190000000004</v>
       </c>
       <c r="V49"/>
@@ -7137,6 +7351,10 @@
         <f t="shared" si="7"/>
         <v>5.2880649825393835</v>
       </c>
+      <c r="R50" s="2">
+        <f t="shared" si="8"/>
+        <v>0.60000799999999987</v>
+      </c>
       <c r="S50">
         <v>6.5458920000000003</v>
       </c>
@@ -7144,7 +7362,7 @@
         <v>7.3616890000000001</v>
       </c>
       <c r="U50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.81579699999999988</v>
       </c>
       <c r="V50"/>
@@ -7200,6 +7418,10 @@
         <f t="shared" si="7"/>
         <v>23.470752854870888</v>
       </c>
+      <c r="R51" s="2">
+        <f t="shared" si="8"/>
+        <v>1.2543640000000003</v>
+      </c>
       <c r="S51">
         <v>3.4449000000000001</v>
       </c>
@@ -7207,7 +7429,7 @@
         <v>3.0485000000000002</v>
       </c>
       <c r="U51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.39639999999999986</v>
       </c>
       <c r="V51"/>
@@ -7263,6 +7485,10 @@
         <f t="shared" si="7"/>
         <v>14.637750354830052</v>
       </c>
+      <c r="R52" s="2">
+        <f t="shared" si="8"/>
+        <v>1.2250519999999998</v>
+      </c>
       <c r="S52">
         <v>4.8829219999999998</v>
       </c>
@@ -7270,7 +7496,7 @@
         <v>6.0089220000000001</v>
       </c>
       <c r="U52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1260000000000003</v>
       </c>
       <c r="V52"/>
@@ -7326,6 +7552,10 @@
         <f t="shared" si="7"/>
         <v>14.782212565274115</v>
       </c>
+      <c r="R53" s="2">
+        <f t="shared" si="8"/>
+        <v>0.4591220000000007</v>
+      </c>
       <c r="S53">
         <v>4.520651</v>
       </c>
@@ -7333,7 +7563,7 @@
         <v>4.7759280000000004</v>
       </c>
       <c r="U53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.25527700000000042</v>
       </c>
       <c r="V53"/>
@@ -7389,6 +7619,10 @@
         <f t="shared" si="7"/>
         <v>8.3797124905570488</v>
       </c>
+      <c r="R54" s="2">
+        <f t="shared" si="8"/>
+        <v>0.51300199999999929</v>
+      </c>
       <c r="S54">
         <v>5.7843809999999998</v>
       </c>
@@ -7396,7 +7630,7 @@
         <v>6.8088280000000001</v>
       </c>
       <c r="U54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.0244470000000003</v>
       </c>
       <c r="V54"/>
@@ -7452,6 +7686,10 @@
         <f t="shared" si="7"/>
         <v>3.6376609457759344</v>
       </c>
+      <c r="R55" s="2">
+        <f t="shared" si="8"/>
+        <v>0.66931999999999992</v>
+      </c>
       <c r="S55">
         <v>6.9225659999999998</v>
       </c>
@@ -7459,7 +7697,7 @@
         <v>8.0734779999999997</v>
       </c>
       <c r="U55">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1509119999999999</v>
       </c>
       <c r="V55"/>
@@ -7515,6 +7753,10 @@
         <f t="shared" si="7"/>
         <v>5.082350671159238E-2</v>
       </c>
+      <c r="R56" s="2">
+        <f t="shared" si="8"/>
+        <v>0.54470899999999922</v>
+      </c>
       <c r="S56">
         <v>7.9653090000000004</v>
       </c>
@@ -7522,7 +7764,7 @@
         <v>9.5583329999999993</v>
       </c>
       <c r="U56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.5930239999999989</v>
       </c>
       <c r="V56"/>
@@ -7578,6 +7820,10 @@
         <f t="shared" si="7"/>
         <v>3.0354235443025823</v>
       </c>
+      <c r="R57" s="2">
+        <f t="shared" si="8"/>
+        <v>0.67988400000000127</v>
+      </c>
       <c r="S57">
         <v>9.8502240000000008</v>
       </c>
@@ -7585,7 +7831,7 @@
         <v>11.796310999999999</v>
       </c>
       <c r="U57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.9460869999999986</v>
       </c>
       <c r="V57"/>
@@ -7641,6 +7887,10 @@
         <f t="shared" si="7"/>
         <v>11.765631935272575</v>
       </c>
+      <c r="R58" s="2">
+        <f t="shared" si="8"/>
+        <v>1.9820729999999998</v>
+      </c>
       <c r="S58">
         <v>12.327113000000001</v>
       </c>
@@ -7648,7 +7898,7 @@
         <v>14.523553</v>
       </c>
       <c r="U58">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.1964399999999991</v>
       </c>
       <c r="V58"/>
@@ -7704,6 +7954,10 @@
         <f t="shared" si="7"/>
         <v>7.6405732880728001</v>
       </c>
+      <c r="R59" s="2">
+        <f t="shared" si="8"/>
+        <v>2.3643970000000003</v>
+      </c>
       <c r="S59">
         <v>14.523591</v>
       </c>
@@ -7711,7 +7965,7 @@
         <v>16.863527000000001</v>
       </c>
       <c r="U59">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.3399360000000016</v>
       </c>
       <c r="V59"/>
@@ -7767,6 +8021,10 @@
         <f t="shared" si="7"/>
         <v>2.3598603430769769</v>
       </c>
+      <c r="R60" s="2">
+        <f t="shared" si="8"/>
+        <v>2.1817769999999985</v>
+      </c>
       <c r="S60">
         <v>14.714471</v>
       </c>
@@ -7774,7 +8032,7 @@
         <v>17.120304000000001</v>
       </c>
       <c r="U60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.4058330000000012</v>
       </c>
       <c r="V60"/>
@@ -7830,6 +8088,10 @@
         <f t="shared" si="7"/>
         <v>0.11201719156731423</v>
       </c>
+      <c r="R61" s="2">
+        <f t="shared" si="8"/>
+        <v>0.33416599999999974</v>
+      </c>
       <c r="S61">
         <v>13.40859</v>
       </c>
@@ -7837,7 +8099,7 @@
         <v>15.784965</v>
       </c>
       <c r="U61">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.3763749999999995</v>
       </c>
       <c r="V61"/>
@@ -7893,6 +8155,10 @@
         <f t="shared" si="7"/>
         <v>1.7088223128171545</v>
       </c>
+      <c r="R62" s="2">
+        <f t="shared" si="8"/>
+        <v>1.2604680000000004</v>
+      </c>
       <c r="S62">
         <v>6.3440430000000001</v>
       </c>
@@ -7900,7 +8166,7 @@
         <v>7.8990039999999997</v>
       </c>
       <c r="U62">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.5549609999999996</v>
       </c>
       <c r="V62"/>
@@ -7956,6 +8222,10 @@
         <f t="shared" si="7"/>
         <v>3.9082771562236585</v>
       </c>
+      <c r="R63" s="2">
+        <f t="shared" si="8"/>
+        <v>1.1889789999999998</v>
+      </c>
       <c r="S63">
         <v>4.6902460000000001</v>
       </c>
@@ -7963,7 +8233,7 @@
         <v>5.8541470000000002</v>
       </c>
       <c r="U63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1639010000000001</v>
       </c>
       <c r="V63"/>
@@ -8019,6 +8289,10 @@
         <f t="shared" si="7"/>
         <v>8.4549304226458837</v>
       </c>
+      <c r="R64" s="2">
+        <f t="shared" si="8"/>
+        <v>0.72412199999999949</v>
+      </c>
       <c r="S64">
         <v>5.0197510000000003</v>
       </c>
@@ -8026,7 +8300,7 @@
         <v>6.4891750000000004</v>
       </c>
       <c r="U64">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.4694240000000001</v>
       </c>
       <c r="V64"/>
@@ -8082,6 +8356,10 @@
         <f t="shared" si="7"/>
         <v>4.1661639372739909</v>
       </c>
+      <c r="R65" s="2">
+        <f t="shared" si="8"/>
+        <v>0.26602199999999954</v>
+      </c>
       <c r="S65">
         <v>5.8286879999999996</v>
       </c>
@@ -8089,7 +8367,7 @@
         <v>8.1289420000000003</v>
       </c>
       <c r="U65">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.3002540000000007</v>
       </c>
       <c r="V65"/>
@@ -8145,6 +8423,10 @@
         <f t="shared" si="7"/>
         <v>2.6475660483157668</v>
       </c>
+      <c r="R66" s="2">
+        <f t="shared" si="8"/>
+        <v>0.96510899999999999</v>
+      </c>
       <c r="S66">
         <v>6.8856330000000003</v>
       </c>
@@ -8152,7 +8434,7 @@
         <v>8.5940560000000001</v>
       </c>
       <c r="U66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.7084229999999998</v>
       </c>
       <c r="V66"/>
@@ -8208,6 +8490,10 @@
         <f t="shared" si="7"/>
         <v>1.6069220854074318</v>
       </c>
+      <c r="R67" s="2">
+        <f t="shared" si="8"/>
+        <v>0.33324699999999918</v>
+      </c>
       <c r="S67">
         <v>7.8171679999999997</v>
       </c>
@@ -8215,7 +8501,7 @@
         <v>9.4432200000000002</v>
       </c>
       <c r="U67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6260520000000005</v>
       </c>
       <c r="V67"/>
@@ -8271,6 +8557,10 @@
         <f t="shared" si="7"/>
         <v>0.80765395121297701</v>
       </c>
+      <c r="R68" s="2">
+        <f t="shared" si="8"/>
+        <v>0.93013499999999993</v>
+      </c>
       <c r="S68">
         <v>9.7518049999999992</v>
       </c>
@@ -8278,7 +8568,7 @@
         <v>11.426868000000001</v>
       </c>
       <c r="U68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6750630000000015</v>
       </c>
       <c r="V68"/>
@@ -8303,36 +8593,40 @@
         <v>11.389341</v>
       </c>
       <c r="J69" s="2">
-        <f t="shared" ref="J69:J111" si="9">I69-H69</f>
+        <f t="shared" ref="J69:J111" si="10">I69-H69</f>
         <v>-1.4981930000000006</v>
       </c>
       <c r="K69" s="2">
-        <f t="shared" ref="K69:K111" si="10">I69-I$2</f>
+        <f t="shared" ref="K69:K111" si="11">I69-I$2</f>
         <v>4.15305612962963</v>
       </c>
       <c r="L69" s="2">
-        <f t="shared" ref="L69:L111" si="11">H69-H$2</f>
+        <f t="shared" ref="L69:L111" si="12">H69-H$2</f>
         <v>4.8274596944444426</v>
       </c>
       <c r="M69" s="2">
-        <f t="shared" ref="M69:M111" si="12">K69*K69</f>
+        <f t="shared" ref="M69:M111" si="13">K69*K69</f>
         <v>17.247875215854243</v>
       </c>
       <c r="N69" s="2">
-        <f t="shared" ref="N69:N111" si="13">L69*L69</f>
+        <f t="shared" ref="N69:N111" si="14">L69*L69</f>
         <v>23.304367101485632</v>
       </c>
       <c r="O69" s="2">
-        <f t="shared" ref="O69:O111" si="14">K69*L69</f>
+        <f t="shared" ref="O69:O111" si="15">K69*L69</f>
         <v>20.048711074552472</v>
       </c>
       <c r="P69" s="2">
-        <f t="shared" ref="P69:P111" si="15">J69*J69</f>
+        <f t="shared" ref="P69:P111" si="16">J69*J69</f>
         <v>2.2445822652490017</v>
       </c>
       <c r="Q69" s="2">
-        <f t="shared" ref="Q69:Q111" si="16">(I69-H$2)*(I69-H$2)</f>
+        <f t="shared" ref="Q69:Q111" si="17">(I69-H$2)*(I69-H$2)</f>
         <v>11.084016722737022</v>
+      </c>
+      <c r="R69" s="2">
+        <f t="shared" ref="R69:R111" si="18">ABS(J69)</f>
+        <v>1.4981930000000006</v>
       </c>
       <c r="S69">
         <v>12.475429999999999</v>
@@ -8341,7 +8635,7 @@
         <v>14.382719</v>
       </c>
       <c r="U69">
-        <f t="shared" ref="U69:U111" si="17">T69-S69</f>
+        <f t="shared" ref="U69:U111" si="19">T69-S69</f>
         <v>1.9072890000000005</v>
       </c>
       <c r="V69"/>
@@ -8366,36 +8660,40 @@
         <v>11.897917</v>
       </c>
       <c r="J70" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.604909000000001</v>
       </c>
       <c r="K70" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.6616321296296297</v>
       </c>
       <c r="L70" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.4427516944444427</v>
       </c>
       <c r="M70" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>21.730814111995276</v>
       </c>
       <c r="N70" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29.623546007377854</v>
       </c>
       <c r="O70" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>25.372106172418324</v>
       </c>
       <c r="P70" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.5757328982810033</v>
       </c>
       <c r="Q70" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14.729036547300572</v>
+      </c>
+      <c r="R70" s="2">
+        <f t="shared" si="18"/>
+        <v>1.604909000000001</v>
       </c>
       <c r="S70">
         <v>14.963448</v>
@@ -8404,7 +8702,7 @@
         <v>17.043074000000001</v>
       </c>
       <c r="U70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.0796260000000011</v>
       </c>
       <c r="V70"/>
@@ -8429,36 +8727,40 @@
         <v>11.168345</v>
       </c>
       <c r="J71" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.3420439999999996</v>
       </c>
       <c r="K71" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.9320601296296305</v>
       </c>
       <c r="L71" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.4503146944444421</v>
       </c>
       <c r="M71" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>15.461096863022986</v>
       </c>
       <c r="N71" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29.705930268477012</v>
       </c>
       <c r="O71" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>21.430965103959494</v>
       </c>
       <c r="P71" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.4851700979359981</v>
       </c>
       <c r="Q71" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.6613467099421371</v>
+      </c>
+      <c r="R71" s="2">
+        <f t="shared" si="18"/>
+        <v>2.3420439999999996</v>
       </c>
       <c r="S71">
         <v>16.450882</v>
@@ -8467,7 +8769,7 @@
         <v>18.608875000000001</v>
       </c>
       <c r="U71">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1579930000000012</v>
       </c>
       <c r="V71"/>
@@ -8492,36 +8794,40 @@
         <v>9.3149300000000004</v>
       </c>
       <c r="J72" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.4910019999999999</v>
       </c>
       <c r="K72" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.0786451296296304</v>
       </c>
       <c r="L72" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7458576944444424</v>
       </c>
       <c r="M72" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.3207655749329827</v>
       </c>
       <c r="N72" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.5397344781397484</v>
       </c>
       <c r="O72" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.7076637232129865</v>
       </c>
       <c r="P72" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.2230869640039996</v>
       </c>
       <c r="Q72" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.5746628138796439</v>
+      </c>
+      <c r="R72" s="2">
+        <f t="shared" si="18"/>
+        <v>1.4910019999999999</v>
       </c>
       <c r="S72">
         <v>15.549884</v>
@@ -8530,7 +8836,7 @@
         <v>17.779147999999999</v>
       </c>
       <c r="U72">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.2292639999999988</v>
       </c>
       <c r="V72"/>
@@ -8555,36 +8861,40 @@
         <v>8.3287630000000004</v>
       </c>
       <c r="J73" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.3272859999999991</v>
       </c>
       <c r="K73" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0924781296296304</v>
       </c>
       <c r="L73" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.5959746944444415</v>
       </c>
       <c r="M73" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.1935084637190556</v>
       </c>
       <c r="N73" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.5471352253070285</v>
       </c>
       <c r="O73" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7435674491228843</v>
       </c>
       <c r="P73" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.7616881257959975</v>
       </c>
       <c r="Q73" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.2193614522258948E-2</v>
+      </c>
+      <c r="R73" s="2">
+        <f t="shared" si="18"/>
+        <v>1.3272859999999991</v>
       </c>
       <c r="S73">
         <v>14.527419</v>
@@ -8593,7 +8903,7 @@
         <v>16.758285999999998</v>
       </c>
       <c r="U73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.2308669999999982</v>
       </c>
       <c r="V73"/>
@@ -8618,36 +8928,40 @@
         <v>5.9748169999999998</v>
       </c>
       <c r="J74" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.0822440000000002</v>
       </c>
       <c r="K74" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.2614678703703701</v>
       </c>
       <c r="L74" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.1675013055555583</v>
       </c>
       <c r="M74" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.5913011879767569</v>
       </c>
       <c r="N74" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10.033064520696167</v>
       </c>
       <c r="O74" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.995701126314537</v>
       </c>
       <c r="P74" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.1712520755360005</v>
       </c>
       <c r="Q74" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.3482980303728258</v>
+      </c>
+      <c r="R74" s="2">
+        <f t="shared" si="18"/>
+        <v>1.0822440000000002</v>
       </c>
       <c r="S74">
         <v>7.187532</v>
@@ -8656,7 +8970,7 @@
         <v>8.207122</v>
       </c>
       <c r="U74">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.01959</v>
       </c>
       <c r="V74"/>
@@ -8681,36 +8995,40 @@
         <v>5.4039159999999997</v>
       </c>
       <c r="J75" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1162109999999998</v>
       </c>
       <c r="K75" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.8323688703703702</v>
       </c>
       <c r="L75" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.7723693055555581</v>
       </c>
       <c r="M75" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.3575756771023868</v>
       </c>
       <c r="N75" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14.230770177497723</v>
       </c>
       <c r="O75" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.9123720830406956</v>
       </c>
       <c r="P75" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2459269965209996</v>
       </c>
       <c r="Q75" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.055176944171774</v>
+      </c>
+      <c r="R75" s="2">
+        <f t="shared" si="18"/>
+        <v>1.1162109999999998</v>
       </c>
       <c r="S75">
         <v>4.2619350000000003</v>
@@ -8719,7 +9037,7 @@
         <v>4.4238860000000004</v>
       </c>
       <c r="U75">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.16195100000000018</v>
       </c>
       <c r="V75"/>
@@ -8744,36 +9062,40 @@
         <v>4.6272169999999999</v>
       </c>
       <c r="J76" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.6744999999999592E-2</v>
       </c>
       <c r="K76" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.60906787037037</v>
       </c>
       <c r="L76" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.4796023055555576</v>
       </c>
       <c r="M76" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.8072351521989782</v>
       </c>
       <c r="N76" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.107632204827553</v>
       </c>
       <c r="O76" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.0785185770916677</v>
       </c>
       <c r="P76" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.1850950249999619E-3</v>
       </c>
       <c r="Q76" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11.784509280306166</v>
+      </c>
+      <c r="R76" s="2">
+        <f t="shared" si="18"/>
+        <v>4.6744999999999592E-2</v>
       </c>
       <c r="S76">
         <v>4.3465230000000004</v>
@@ -8782,7 +9104,7 @@
         <v>4.3064270000000002</v>
       </c>
       <c r="U76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-4.0096000000000132E-2</v>
       </c>
       <c r="V76"/>
@@ -8807,36 +9129,40 @@
         <v>5.3779450000000004</v>
       </c>
       <c r="J77" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-7.1200999999999404E-2</v>
       </c>
       <c r="K77" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.8583398703703695</v>
       </c>
       <c r="L77" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.6109283055555581</v>
       </c>
       <c r="M77" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.4534270738081618</v>
       </c>
       <c r="N77" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.8169466167512178</v>
       </c>
       <c r="O77" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.8519921688924441</v>
       </c>
       <c r="P77" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.0695824009999151E-3</v>
       </c>
       <c r="Q77" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.1938176117199371</v>
+      </c>
+      <c r="R77" s="2">
+        <f t="shared" si="18"/>
+        <v>7.1200999999999404E-2</v>
       </c>
       <c r="S77">
         <v>5.355829</v>
@@ -8845,7 +9171,7 @@
         <v>6.6809029999999998</v>
       </c>
       <c r="U77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.3250739999999999</v>
       </c>
       <c r="V77"/>
@@ -8870,36 +9196,40 @@
         <v>5.659497</v>
       </c>
       <c r="J78" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.19680599999999959</v>
       </c>
       <c r="K78" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.5767878703703699</v>
       </c>
       <c r="L78" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.5973833055555575</v>
       </c>
       <c r="M78" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.4862599881471263</v>
       </c>
       <c r="N78" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.7464000359787146</v>
       </c>
       <c r="O78" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.095522490902499</v>
       </c>
       <c r="P78" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.8732601635999842E-2</v>
       </c>
       <c r="Q78" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.7627713999483827</v>
+      </c>
+      <c r="R78" s="2">
+        <f t="shared" si="18"/>
+        <v>0.19680599999999959</v>
       </c>
       <c r="S78">
         <v>5.5344850000000001</v>
@@ -8908,7 +9238,7 @@
         <v>6.7397119999999999</v>
       </c>
       <c r="U78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.2052269999999998</v>
       </c>
       <c r="V78"/>
@@ -8933,36 +9263,40 @@
         <v>6.7848269999999999</v>
       </c>
       <c r="J79" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.0356319999999997</v>
       </c>
       <c r="K79" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.45145787037037</v>
       </c>
       <c r="L79" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.23961530555555832</v>
       </c>
       <c r="M79" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.2038142087193498</v>
       </c>
       <c r="N79" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.741549465648358E-2</v>
       </c>
       <c r="O79" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.10817621555425784</v>
       </c>
       <c r="P79" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0725336394239993</v>
       </c>
       <c r="Q79" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.6262556903267107</v>
+      </c>
+      <c r="R79" s="2">
+        <f t="shared" si="18"/>
+        <v>1.0356319999999997</v>
       </c>
       <c r="S79">
         <v>7.4366459999999996</v>
@@ -8971,7 +9305,7 @@
         <v>8.7652110000000008</v>
       </c>
       <c r="U79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.3285650000000011</v>
       </c>
       <c r="V79"/>
@@ -8996,36 +9330,40 @@
         <v>8.7718749999999996</v>
       </c>
       <c r="J80" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.8169789999999999</v>
       </c>
       <c r="K80" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.5355901296296297</v>
       </c>
       <c r="L80" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.5287796944444416</v>
       </c>
       <c r="M80" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.358037046215943</v>
       </c>
       <c r="N80" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.3371673541456404</v>
       </c>
       <c r="O80" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.3475790091670858</v>
       </c>
       <c r="P80" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.66745468644099981</v>
       </c>
       <c r="Q80" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.50666022861158944</v>
+      </c>
+      <c r="R80" s="2">
+        <f t="shared" si="18"/>
+        <v>0.8169789999999999</v>
       </c>
       <c r="S80">
         <v>9.1137759999999997</v>
@@ -9034,7 +9372,7 @@
         <v>10.81246</v>
       </c>
       <c r="U80">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.6986840000000001</v>
       </c>
       <c r="V80"/>
@@ -9059,36 +9397,40 @@
         <v>10.353471000000001</v>
       </c>
       <c r="J81" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.0071569999999994</v>
       </c>
       <c r="K81" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.1171861296296308</v>
       </c>
       <c r="L81" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.3005536944444422</v>
       </c>
       <c r="M81" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9.7168493667553584</v>
       </c>
       <c r="N81" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10.893654689910857</v>
       </c>
       <c r="O81" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>10.28844019642005</v>
       </c>
       <c r="P81" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0143652226489988</v>
       </c>
       <c r="Q81" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.2596683980886967</v>
+      </c>
+      <c r="R81" s="2">
+        <f t="shared" si="18"/>
+        <v>1.0071569999999994</v>
       </c>
       <c r="S81">
         <v>10.387589</v>
@@ -9097,7 +9439,7 @@
         <v>12.286628</v>
       </c>
       <c r="U81">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.8990390000000001</v>
       </c>
       <c r="V81"/>
@@ -9122,36 +9464,40 @@
         <v>11.011625</v>
       </c>
       <c r="J82" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.193441</v>
       </c>
       <c r="K82" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.7753401296296305</v>
       </c>
       <c r="L82" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.1449916944444425</v>
       </c>
       <c r="M82" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14.253193094391875</v>
       </c>
       <c r="N82" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>17.180956147013411</v>
       </c>
       <c r="O82" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15.648753481017623</v>
       </c>
       <c r="P82" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.4243014204809998</v>
       </c>
       <c r="Q82" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.7116515018754708</v>
+      </c>
+      <c r="R82" s="2">
+        <f t="shared" si="18"/>
+        <v>1.193441</v>
       </c>
       <c r="S82">
         <v>12.385052</v>
@@ -9160,7 +9506,7 @@
         <v>14.413005</v>
       </c>
       <c r="U82">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.0279530000000001</v>
       </c>
       <c r="V82"/>
@@ -9185,36 +9531,40 @@
         <v>10.872294999999999</v>
       </c>
       <c r="J83" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.515784</v>
       </c>
       <c r="K83" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.6360101296296294</v>
       </c>
       <c r="L83" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.3280046944444415</v>
       </c>
       <c r="M83" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>13.220569662769275</v>
       </c>
       <c r="N83" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28.387634024022006</v>
       </c>
       <c r="O83" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19.372679039714207</v>
       </c>
       <c r="P83" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6.3291691346560004</v>
       </c>
       <c r="Q83" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.9085852342615768</v>
+      </c>
+      <c r="R83" s="2">
+        <f t="shared" si="18"/>
+        <v>2.515784</v>
       </c>
       <c r="S83">
         <v>14.474914999999999</v>
@@ -9223,7 +9573,7 @@
         <v>16.593639</v>
       </c>
       <c r="U83">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1187240000000003</v>
       </c>
       <c r="V83"/>
@@ -9248,36 +9598,40 @@
         <v>9.0363220000000002</v>
       </c>
       <c r="J84" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.6288249999999991</v>
       </c>
       <c r="K84" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.8000371296296303</v>
       </c>
       <c r="L84" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.6050726944444413</v>
       </c>
       <c r="M84" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.2401336680452784</v>
       </c>
       <c r="N84" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.7864037433400215</v>
       </c>
       <c r="O84" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.6892275753842991</v>
       </c>
       <c r="P84" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.653070880624997</v>
       </c>
       <c r="Q84" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.95305956090808908</v>
+      </c>
+      <c r="R84" s="2">
+        <f t="shared" si="18"/>
+        <v>1.6288249999999991</v>
       </c>
       <c r="S84">
         <v>14.355328</v>
@@ -9286,7 +9640,7 @@
         <v>16.534609</v>
       </c>
       <c r="U84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1792809999999996</v>
       </c>
       <c r="V84"/>
@@ -9311,36 +9665,40 @@
         <v>8.2622250000000008</v>
       </c>
       <c r="J85" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1933520000000009</v>
       </c>
       <c r="K85" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0259401296296309</v>
       </c>
       <c r="L85" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.99120130555555797</v>
       </c>
       <c r="M85" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0525531495844638</v>
       </c>
       <c r="N85" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.98248002813504254</v>
       </c>
       <c r="O85" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-1.0169131959107285</v>
       </c>
       <c r="P85" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.424088995904002</v>
       </c>
       <c r="Q85" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.0864903264370513E-2</v>
+      </c>
+      <c r="R85" s="2">
+        <f t="shared" si="18"/>
+        <v>1.1933520000000009</v>
       </c>
       <c r="S85">
         <v>10.698161000000001</v>
@@ -9349,7 +9707,7 @@
         <v>12.883421999999999</v>
       </c>
       <c r="U85">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1852609999999988</v>
       </c>
       <c r="V85"/>
@@ -9374,36 +9732,40 @@
         <v>7.2404169999999999</v>
       </c>
       <c r="J86" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1280739999999998</v>
       </c>
       <c r="K86" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.1321296296299437E-3</v>
       </c>
       <c r="L86" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-1.9477313055555578</v>
       </c>
       <c r="M86" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.7074495276065697E-5</v>
       </c>
       <c r="N86" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.793657238641158</v>
       </c>
       <c r="O86" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-8.048278238243934E-3</v>
       </c>
       <c r="P86" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2725509494759994</v>
       </c>
       <c r="Q86" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.6718380985505974</v>
+      </c>
+      <c r="R86" s="2">
+        <f t="shared" si="18"/>
+        <v>1.1280739999999998</v>
       </c>
       <c r="S86">
         <v>5.870679</v>
@@ -9412,7 +9774,7 @@
         <v>7.5376799999999999</v>
       </c>
       <c r="U86">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.667001</v>
       </c>
       <c r="V86"/>
@@ -9437,36 +9799,40 @@
         <v>4.67211</v>
       </c>
       <c r="J87" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.99129500000000004</v>
       </c>
       <c r="K87" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.56417487037037</v>
       </c>
       <c r="L87" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-4.379259305555558</v>
       </c>
       <c r="M87" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.5749927658389034</v>
       </c>
       <c r="N87" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19.177912065294947</v>
       </c>
       <c r="O87" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11.22918666214116</v>
       </c>
       <c r="P87" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.98266577702500002</v>
       </c>
       <c r="Q87" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11.478302135718554</v>
+      </c>
+      <c r="R87" s="2">
+        <f t="shared" si="18"/>
+        <v>0.99129500000000004</v>
       </c>
       <c r="S87">
         <v>3.4921540000000002</v>
@@ -9475,7 +9841,7 @@
         <v>2.3836870000000001</v>
       </c>
       <c r="U87">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-1.1084670000000001</v>
       </c>
       <c r="V87"/>
@@ -9500,36 +9866,40 @@
         <v>3.6666099999999999</v>
       </c>
       <c r="J88" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.44046200000000013</v>
       </c>
       <c r="K88" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-3.56967487037037</v>
       </c>
       <c r="L88" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-4.8339263055555577</v>
       </c>
       <c r="M88" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12.742578680153718</v>
       </c>
       <c r="N88" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>23.366843527542002</v>
       </c>
       <c r="O88" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17.255545258163956</v>
       </c>
       <c r="P88" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.19400677344400011</v>
       </c>
       <c r="Q88" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>19.302528604190776</v>
+      </c>
+      <c r="R88" s="2">
+        <f t="shared" si="18"/>
+        <v>0.44046200000000013</v>
       </c>
       <c r="S88">
         <v>1.1970860000000001</v>
@@ -9538,7 +9908,7 @@
         <v>-2.3392900000000001</v>
       </c>
       <c r="U88">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-3.5363760000000002</v>
       </c>
       <c r="V88"/>
@@ -9563,36 +9933,40 @@
         <v>4.7065109999999999</v>
       </c>
       <c r="J89" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.39239499999999961</v>
       </c>
       <c r="K89" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.52977387037037</v>
       </c>
       <c r="L89" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.7459583055555576</v>
       </c>
       <c r="M89" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.3997558352086816</v>
       </c>
       <c r="N89" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14.032203626960664</v>
       </c>
       <c r="O89" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.4764274408913156</v>
       </c>
       <c r="P89" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.1539738360249997</v>
       </c>
       <c r="Q89" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11.246386844368722</v>
+      </c>
+      <c r="R89" s="2">
+        <f t="shared" si="18"/>
+        <v>0.39239499999999961</v>
       </c>
       <c r="S89">
         <v>2.6418699999999999</v>
@@ -9601,7 +9975,7 @@
         <v>1.3647229999999999</v>
       </c>
       <c r="U89">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-1.277147</v>
       </c>
       <c r="V89"/>
@@ -9626,36 +10000,40 @@
         <v>4.946485</v>
       </c>
       <c r="J90" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.79513699999999954</v>
       </c>
       <c r="K90" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.2897998703703699</v>
       </c>
       <c r="L90" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.3184523055555584</v>
       </c>
       <c r="M90" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.243183446348163</v>
       </c>
       <c r="N90" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.3752210931358846</v>
       </c>
       <c r="O90" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.3087917887210025</v>
       </c>
       <c r="P90" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.63224284876899928</v>
       </c>
       <c r="Q90" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.694438363669942</v>
+      </c>
+      <c r="R90" s="2">
+        <f t="shared" si="18"/>
+        <v>0.79513699999999954</v>
       </c>
       <c r="S90">
         <v>4.3188110000000002</v>
@@ -9664,7 +10042,7 @@
         <v>4.5756379999999996</v>
       </c>
       <c r="U90">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.25682699999999947</v>
       </c>
       <c r="V90"/>
@@ -9689,36 +10067,40 @@
         <v>5.5992629999999997</v>
       </c>
       <c r="J91" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.5397850000000002</v>
       </c>
       <c r="K91" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.6370218703703703</v>
       </c>
       <c r="L91" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.92102630555555809</v>
       </c>
       <c r="M91" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.6798406040709053</v>
       </c>
       <c r="N91" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.8482894555253202</v>
       </c>
       <c r="O91" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.5077402053808719</v>
       </c>
       <c r="P91" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.3709378462250004</v>
       </c>
       <c r="Q91" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.0555922815500516</v>
+      </c>
+      <c r="R91" s="2">
+        <f t="shared" si="18"/>
+        <v>1.5397850000000002</v>
       </c>
       <c r="S91">
         <v>5.710909</v>
@@ -9727,7 +10109,7 @@
         <v>7.86172</v>
       </c>
       <c r="U91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.150811</v>
       </c>
       <c r="V91"/>
@@ -9752,36 +10134,40 @@
         <v>7.0140260000000003</v>
       </c>
       <c r="J92" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.8254879999999991</v>
       </c>
       <c r="K92" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.22225887037036962</v>
       </c>
       <c r="L92" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.7794396944444415</v>
       </c>
       <c r="M92" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.9399005458312766E-2</v>
       </c>
       <c r="N92" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.1664056261645275</v>
       </c>
       <c r="O92" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.39549625637941727</v>
       </c>
       <c r="P92" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.9833824381439946</v>
       </c>
       <c r="Q92" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.0942170575556531</v>
+      </c>
+      <c r="R92" s="2">
+        <f t="shared" si="18"/>
+        <v>2.8254879999999991</v>
       </c>
       <c r="S92">
         <v>7.193924</v>
@@ -9790,7 +10176,7 @@
         <v>9.5902989999999999</v>
       </c>
       <c r="U92">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.3963749999999999</v>
       </c>
       <c r="V92"/>
@@ -9815,36 +10201,40 @@
         <v>9.7849989999999991</v>
       </c>
       <c r="J93" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.9001920000000005</v>
       </c>
       <c r="K93" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.5487141296296292</v>
       </c>
       <c r="L93" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.6251166944444417</v>
       </c>
       <c r="M93" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.495943714573718</v>
       </c>
       <c r="N93" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>21.391704437228679</v>
       </c>
       <c r="O93" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11.788100270316432</v>
       </c>
       <c r="P93" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.4111136368640036</v>
       </c>
       <c r="Q93" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.9753652015042489</v>
+      </c>
+      <c r="R93" s="2">
+        <f t="shared" si="18"/>
+        <v>2.9001920000000005</v>
       </c>
       <c r="S93">
         <v>8.9577299999999997</v>
@@ -9853,7 +10243,7 @@
         <v>11.902104</v>
       </c>
       <c r="U93">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.9443739999999998</v>
       </c>
       <c r="V93"/>
@@ -9878,36 +10268,40 @@
         <v>11.298373</v>
       </c>
       <c r="J94" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4.5415700000000001</v>
       </c>
       <c r="K94" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.0620881296296298</v>
       </c>
       <c r="L94" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.779868694444442</v>
       </c>
       <c r="M94" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16.500559972877944</v>
       </c>
       <c r="N94" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>60.526356902796664</v>
       </c>
       <c r="O94" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>31.602512273779933</v>
       </c>
       <c r="P94" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>20.625858064900001</v>
       </c>
       <c r="Q94" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>10.486578434440576</v>
+      </c>
+      <c r="R94" s="2">
+        <f t="shared" si="18"/>
+        <v>4.5415700000000001</v>
       </c>
       <c r="S94">
         <v>11.752560000000001</v>
@@ -9916,7 +10310,7 @@
         <v>14.932577999999999</v>
       </c>
       <c r="U94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>3.1800179999999987</v>
       </c>
       <c r="V94"/>
@@ -9941,36 +10335,40 @@
         <v>10.501163</v>
       </c>
       <c r="J95" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-3.1274119999999996</v>
       </c>
       <c r="K95" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.2648781296296301</v>
       </c>
       <c r="L95" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.5685006944444417</v>
       </c>
       <c r="M95" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>10.659429201333872</v>
       </c>
       <c r="N95" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>31.008199984028231</v>
       </c>
       <c r="O95" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18.180476132119065</v>
       </c>
       <c r="P95" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.7807058177439981</v>
       </c>
       <c r="Q95" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.9589140141444705</v>
+      </c>
+      <c r="R95" s="2">
+        <f t="shared" si="18"/>
+        <v>3.1274119999999996</v>
       </c>
       <c r="S95">
         <v>13.397656</v>
@@ -9979,7 +10377,7 @@
         <v>16.595585</v>
       </c>
       <c r="U95">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>3.1979290000000002</v>
       </c>
       <c r="V95"/>
@@ -10004,36 +10402,40 @@
         <v>9.2247319999999995</v>
       </c>
       <c r="J96" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.2991159999999997</v>
       </c>
       <c r="K96" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.9884471296296296</v>
       </c>
       <c r="L96" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.4637736944444413</v>
       </c>
       <c r="M96" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.9539219873323126</v>
       </c>
       <c r="N96" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.0701808174364107</v>
       </c>
       <c r="O96" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.899083730775037</v>
       </c>
       <c r="P96" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.6877023814559993</v>
       </c>
       <c r="Q96" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.3564275452286423</v>
+      </c>
+      <c r="R96" s="2">
+        <f t="shared" si="18"/>
+        <v>1.2991159999999997</v>
       </c>
       <c r="S96">
         <v>13.115736999999999</v>
@@ -10042,7 +10444,7 @@
         <v>16.301480999999999</v>
       </c>
       <c r="U96">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>3.1857439999999997</v>
       </c>
       <c r="V96"/>
@@ -10067,36 +10469,40 @@
         <v>7.2264099999999996</v>
       </c>
       <c r="J97" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.34260099999999927</v>
       </c>
       <c r="K97" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-9.8748703703703811E-3</v>
       </c>
       <c r="L97" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-1.1762653055555576</v>
       </c>
       <c r="M97" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9.7513064831618873E-5</v>
       </c>
       <c r="N97" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.3836000690537094</v>
       </c>
       <c r="O97" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.1615467413525239E-2</v>
       </c>
       <c r="P97" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.1173754452009995</v>
       </c>
       <c r="Q97" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.69499617435743144</v>
+      </c>
+      <c r="R97" s="2">
+        <f t="shared" si="18"/>
+        <v>0.34260099999999927</v>
       </c>
       <c r="S97">
         <v>9.924175</v>
@@ -10105,7 +10511,7 @@
         <v>12.758827</v>
       </c>
       <c r="U97">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.8346520000000002</v>
       </c>
       <c r="V97"/>
@@ -10130,36 +10536,40 @@
         <v>6.0619870000000002</v>
       </c>
       <c r="J98" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.8802200000000004</v>
       </c>
       <c r="K98" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.1742978703703697</v>
       </c>
       <c r="L98" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.8783073055555581</v>
       </c>
       <c r="M98" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.3789754883563856</v>
       </c>
       <c r="N98" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15.041267556325613</v>
       </c>
       <c r="O98" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.554288009555739</v>
       </c>
       <c r="P98" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.5352272484000018</v>
       </c>
       <c r="Q98" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3.9923528806222688</v>
+      </c>
+      <c r="R98" s="2">
+        <f t="shared" si="18"/>
+        <v>1.8802200000000004</v>
       </c>
       <c r="S98">
         <v>4.5283889999999998</v>
@@ -10168,7 +10578,7 @@
         <v>5.2282070000000003</v>
       </c>
       <c r="U98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.6998180000000005</v>
       </c>
       <c r="V98"/>
@@ -10193,36 +10603,40 @@
         <v>4.5872989999999998</v>
       </c>
       <c r="J99" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.765212</v>
       </c>
       <c r="K99" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.6489858703703701</v>
       </c>
       <c r="L99" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-4.2379873055555581</v>
       </c>
       <c r="M99" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.0171261414218673</v>
       </c>
       <c r="N99" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>17.96053640205006</v>
       </c>
       <c r="O99" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11.226368491225671</v>
       </c>
       <c r="P99" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.58554940494399998</v>
       </c>
       <c r="Q99" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12.0601683228765</v>
+      </c>
+      <c r="R99" s="2">
+        <f t="shared" si="18"/>
+        <v>0.765212</v>
       </c>
       <c r="S99">
         <v>2.3634759999999999</v>
@@ -10231,7 +10645,7 @@
         <v>1.344606</v>
       </c>
       <c r="U99">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-1.0188699999999999</v>
       </c>
       <c r="V99"/>
@@ -10256,36 +10670,40 @@
         <v>4.9552849999999999</v>
       </c>
       <c r="J100" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.21234500000000001</v>
       </c>
       <c r="K100" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.28099987037037</v>
       </c>
       <c r="L100" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.892444305555558</v>
       </c>
       <c r="M100" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.2029604086296448</v>
       </c>
       <c r="N100" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.3662340607407746</v>
       </c>
       <c r="O100" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.5976650860257422</v>
       </c>
       <c r="P100" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.5090399025000005E-2</v>
       </c>
       <c r="Q100" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.6397166318921634</v>
+      </c>
+      <c r="R100" s="2">
+        <f t="shared" si="18"/>
+        <v>0.21234500000000001</v>
       </c>
       <c r="S100">
         <v>4.4663490000000001</v>
@@ -10294,7 +10712,7 @@
         <v>5.4185150000000002</v>
       </c>
       <c r="U100">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.95216600000000007</v>
       </c>
       <c r="V100"/>
@@ -10319,36 +10737,40 @@
         <v>4.2978680000000002</v>
       </c>
       <c r="J101" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.28220299999999998</v>
       </c>
       <c r="K101" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.9384168703703697</v>
       </c>
       <c r="L101" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.4800033055555577</v>
       </c>
       <c r="M101" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.6342937040771979</v>
       </c>
       <c r="N101" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.110423006677609</v>
       </c>
       <c r="O101" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>10.225700421989103</v>
       </c>
       <c r="P101" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.9638533208999995E-2</v>
       </c>
       <c r="Q101" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14.154196285561998</v>
+      </c>
+      <c r="R101" s="2">
+        <f t="shared" si="18"/>
+        <v>0.28220299999999998</v>
       </c>
       <c r="S101">
         <v>4.6956059999999997</v>
@@ -10357,7 +10779,7 @@
         <v>5.7108840000000001</v>
       </c>
       <c r="U101">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.0152780000000003</v>
       </c>
       <c r="V101"/>
@@ -10382,36 +10804,40 @@
         <v>4.6569880000000001</v>
       </c>
       <c r="J102" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.94466599999999978</v>
       </c>
       <c r="K102" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.5792968703703698</v>
       </c>
       <c r="L102" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.458420305555558</v>
       </c>
       <c r="M102" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.6527723455023846</v>
       </c>
       <c r="N102" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.0438303987678834</v>
       </c>
       <c r="O102" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.3409958001744187</v>
       </c>
       <c r="P102" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.8923938515559996</v>
       </c>
       <c r="Q102" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11.580996403059775</v>
+      </c>
+      <c r="R102" s="2">
+        <f t="shared" si="18"/>
+        <v>0.94466599999999978</v>
       </c>
       <c r="S102">
         <v>5.3733880000000003</v>
@@ -10420,7 +10846,7 @@
         <v>5.9636950000000004</v>
       </c>
       <c r="U102">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.59030700000000014</v>
       </c>
       <c r="V102"/>
@@ -10445,36 +10871,40 @@
         <v>5.8367180000000003</v>
       </c>
       <c r="J103" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.0616019999999997</v>
       </c>
       <c r="K103" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.3995668703703696</v>
       </c>
       <c r="L103" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-1.1617543055555579</v>
       </c>
       <c r="M103" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.958787424638311</v>
       </c>
       <c r="N103" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.3496730664768766</v>
       </c>
       <c r="O103" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6259528375656944</v>
       </c>
       <c r="P103" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.1269988064039993</v>
       </c>
       <c r="Q103" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.9433132614536586</v>
+      </c>
+      <c r="R103" s="2">
+        <f t="shared" si="18"/>
+        <v>1.0616019999999997</v>
       </c>
       <c r="S103">
         <v>6.4953919999999998</v>
@@ -10483,7 +10913,7 @@
         <v>7.5892429999999997</v>
       </c>
       <c r="U103">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.0938509999999999</v>
       </c>
       <c r="V103"/>
@@ -10508,36 +10938,40 @@
         <v>8.8799700000000001</v>
       </c>
       <c r="J104" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.5441330000000004</v>
       </c>
       <c r="K104" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.6436851296296302</v>
       </c>
       <c r="L104" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.3640286944444426</v>
       </c>
       <c r="M104" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.7017008053655744</v>
       </c>
       <c r="N104" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.5886316681566957</v>
       </c>
       <c r="O104" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.885718811076079</v>
       </c>
       <c r="P104" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.3843467216890013</v>
       </c>
       <c r="Q104" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.6722289497685342</v>
+      </c>
+      <c r="R104" s="2">
+        <f t="shared" si="18"/>
+        <v>1.5441330000000004</v>
       </c>
       <c r="S104">
         <v>9.6104040000000008</v>
@@ -10546,7 +10980,7 @@
         <v>11.136310999999999</v>
       </c>
       <c r="U104">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.5259069999999983</v>
       </c>
       <c r="V104"/>
@@ -10571,36 +11005,40 @@
         <v>10.157683</v>
       </c>
       <c r="J105" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.0657920000000001</v>
       </c>
       <c r="K105" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.9213981296296305</v>
       </c>
       <c r="L105" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.1634006944444426</v>
       </c>
       <c r="M105" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.534567031803503</v>
       </c>
       <c r="N105" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10.007103953611582</v>
       </c>
       <c r="O105" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.2415528720190689</v>
       </c>
       <c r="P105" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.1359125872640001</v>
       </c>
       <c r="Q105" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.3999622350089185</v>
+      </c>
+      <c r="R105" s="2">
+        <f t="shared" si="18"/>
+        <v>1.0657920000000001</v>
       </c>
       <c r="S105">
         <v>10.771552</v>
@@ -10609,7 +11047,7 @@
         <v>12.600471000000001</v>
       </c>
       <c r="U105">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.8289190000000008</v>
       </c>
       <c r="V105"/>
@@ -10634,36 +11072,40 @@
         <v>11.548427</v>
       </c>
       <c r="J106" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.2680699999999998</v>
       </c>
       <c r="K106" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.3121421296296303</v>
       </c>
       <c r="L106" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.7564226944444421</v>
       </c>
       <c r="M106" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>18.594569746126762</v>
       </c>
       <c r="N106" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.136402237115014</v>
       </c>
       <c r="O106" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>24.822512816669992</v>
       </c>
       <c r="P106" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.1441415248999993</v>
       </c>
       <c r="Q106" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12.1686045208378</v>
+      </c>
+      <c r="R106" s="2">
+        <f t="shared" si="18"/>
+        <v>2.2680699999999998</v>
       </c>
       <c r="S106">
         <v>13.215975</v>
@@ -10672,7 +11114,7 @@
         <v>15.246349</v>
       </c>
       <c r="U106">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.0303740000000001</v>
       </c>
       <c r="V106"/>
@@ -10697,36 +11139,40 @@
         <v>10.903589</v>
       </c>
       <c r="J107" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.4428380000000001</v>
       </c>
       <c r="K107" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.6673041296296303</v>
       </c>
       <c r="L107" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.2863526944444423</v>
       </c>
       <c r="M107" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>13.449119579198539</v>
       </c>
       <c r="N107" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27.945524810060014</v>
       </c>
       <c r="O107" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19.386663067014826</v>
       </c>
       <c r="P107" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.967457494244</v>
       </c>
       <c r="Q107" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.0855758175214696</v>
+      </c>
+      <c r="R107" s="2">
+        <f t="shared" si="18"/>
+        <v>2.4428380000000001</v>
       </c>
       <c r="S107">
         <v>15.243527</v>
@@ -10735,7 +11181,7 @@
         <v>17.401871</v>
       </c>
       <c r="U107">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.1583439999999996</v>
       </c>
       <c r="V107"/>
@@ -10760,36 +11206,40 @@
         <v>8.9095630000000003</v>
       </c>
       <c r="J108" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.8926009999999991</v>
       </c>
       <c r="K108" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.6732781296296304</v>
       </c>
       <c r="L108" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7420896944444415</v>
       </c>
       <c r="M108" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.7998596990968343</v>
       </c>
       <c r="N108" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.519055892378411</v>
       </c>
       <c r="O108" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.5882787151966795</v>
       </c>
       <c r="P108" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.5819385452009964</v>
       </c>
       <c r="Q108" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.72163104198892325</v>
+      </c>
+      <c r="R108" s="2">
+        <f t="shared" si="18"/>
+        <v>1.8926009999999991</v>
       </c>
       <c r="S108">
         <v>14.913529</v>
@@ -10798,7 +11248,7 @@
         <v>17.110749999999999</v>
       </c>
       <c r="U108">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.197220999999999</v>
       </c>
       <c r="V108"/>
@@ -10823,36 +11273,40 @@
         <v>7.4504200000000003</v>
       </c>
       <c r="J109" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.093659999999999</v>
       </c>
       <c r="K109" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.21413512962963033</v>
       </c>
       <c r="L109" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.4840056944444413</v>
       </c>
       <c r="M109" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5853853741498585E-2</v>
       </c>
       <c r="N109" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.23426151225464589</v>
       </c>
       <c r="O109" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.10364262212133969</v>
       </c>
       <c r="P109" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.1960921955999977</v>
       </c>
       <c r="Q109" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.37167837228242928</v>
+      </c>
+      <c r="R109" s="2">
+        <f t="shared" si="18"/>
+        <v>1.093659999999999</v>
       </c>
       <c r="S109">
         <v>13.524543</v>
@@ -10861,7 +11315,7 @@
         <v>15.616877000000001</v>
       </c>
       <c r="U109">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>2.092334000000001</v>
       </c>
       <c r="V109"/>
@@ -10886,36 +11340,40 @@
         <v>5.8304580000000001</v>
       </c>
       <c r="J110" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-3.2573000000000185E-2</v>
       </c>
       <c r="K110" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.4058268703703698</v>
       </c>
       <c r="L110" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.1970433055555576</v>
       </c>
       <c r="M110" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.9763491894553484</v>
       </c>
       <c r="N110" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.8269992864864912</v>
       </c>
       <c r="O110" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.0886625143173418</v>
       </c>
       <c r="P110" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.061000329000012E-3</v>
       </c>
       <c r="Q110" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.9711888699992146</v>
+      </c>
+      <c r="R110" s="2">
+        <f t="shared" si="18"/>
+        <v>3.2573000000000185E-2</v>
       </c>
       <c r="S110">
         <v>7.9147090000000002</v>
@@ -10924,7 +11382,7 @@
         <v>9.3853279999999994</v>
       </c>
       <c r="U110">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.4706189999999992</v>
       </c>
       <c r="V110"/>
@@ -10949,36 +11407,40 @@
         <v>4.8333740000000001</v>
       </c>
       <c r="J111" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.32102499999999967</v>
       </c>
       <c r="K111" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-2.4029108703703699</v>
       </c>
       <c r="L111" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.5477253055555575</v>
       </c>
       <c r="M111" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.7739806509440887</v>
       </c>
       <c r="N111" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.586354843679274</v>
       </c>
       <c r="O111" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8.5248677018074908</v>
       </c>
       <c r="P111" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.10305705062499979</v>
       </c>
       <c r="Q111" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>10.411594861872331</v>
+      </c>
+      <c r="R111" s="2">
+        <f t="shared" si="18"/>
+        <v>0.32102499999999967</v>
       </c>
       <c r="S111">
         <v>4.2786520000000001</v>
@@ -10987,7 +11449,7 @@
         <v>4.3472080000000002</v>
       </c>
       <c r="U111">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>6.8556000000000061E-2</v>
       </c>
       <c r="V111"/>
@@ -36454,40 +36916,40 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>